<commit_message>
replace it questions continued
</commit_message>
<xml_diff>
--- a/public/docs/Grammar_replaceit_exercise.xlsx
+++ b/public/docs/Grammar_replaceit_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFA27A1-C2B9-4F41-A424-6F47FEC4AA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C339AD-E391-44A3-AF31-DF7A91C00E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
+    <workbookView xWindow="1560" yWindow="1020" windowWidth="14220" windowHeight="8880" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2692" uniqueCount="251">
   <si>
     <t>{beginning: "</t>
   </si>
@@ -186,6 +186,609 @@
   </si>
   <si>
     <t>LESSON 30</t>
+  </si>
+  <si>
+    <t>Він</t>
+  </si>
+  <si>
+    <t>Ми</t>
+  </si>
+  <si>
+    <t>Вона</t>
+  </si>
+  <si>
+    <t>Ти</t>
+  </si>
+  <si>
+    <t>Вони</t>
+  </si>
+  <si>
+    <t>Ви</t>
+  </si>
+  <si>
+    <t>Воно</t>
+  </si>
+  <si>
+    <t>He</t>
+  </si>
+  <si>
+    <t>We</t>
+  </si>
+  <si>
+    <t>She</t>
+  </si>
+  <si>
+    <t>You</t>
+  </si>
+  <si>
+    <t>They</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>likes ice-cream</t>
+  </si>
+  <si>
+    <t>learn English</t>
+  </si>
+  <si>
+    <t>goes to town</t>
+  </si>
+  <si>
+    <t>help people</t>
+  </si>
+  <si>
+    <t>look in the window</t>
+  </si>
+  <si>
+    <t>want peace</t>
+  </si>
+  <si>
+    <t>will find the key</t>
+  </si>
+  <si>
+    <t>knows something</t>
+  </si>
+  <si>
+    <t>take our time</t>
+  </si>
+  <si>
+    <t>want</t>
+  </si>
+  <si>
+    <t>more juice</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>What do you</t>
+  </si>
+  <si>
+    <t>eat</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>talk</t>
+  </si>
+  <si>
+    <t>about school</t>
+  </si>
+  <si>
+    <t>All kids</t>
+  </si>
+  <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>runs</t>
+  </si>
+  <si>
+    <t>fast</t>
+  </si>
+  <si>
+    <t>Many birds</t>
+  </si>
+  <si>
+    <t>sing</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>homework</t>
+  </si>
+  <si>
+    <t>Most people</t>
+  </si>
+  <si>
+    <t>smile</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>goes</t>
+  </si>
+  <si>
+    <t>хочу</t>
+  </si>
+  <si>
+    <t>має</t>
+  </si>
+  <si>
+    <t>many friends</t>
+  </si>
+  <si>
+    <t>їсте</t>
+  </si>
+  <si>
+    <t>говоримо</t>
+  </si>
+  <si>
+    <t>граються</t>
+  </si>
+  <si>
+    <t>бігає</t>
+  </si>
+  <si>
+    <t>співають</t>
+  </si>
+  <si>
+    <t>роблять</t>
+  </si>
+  <si>
+    <t>посміхаються</t>
+  </si>
+  <si>
+    <t>йде</t>
+  </si>
+  <si>
+    <t>will like</t>
+  </si>
+  <si>
+    <t>this book</t>
+  </si>
+  <si>
+    <t>will use</t>
+  </si>
+  <si>
+    <t>that pan</t>
+  </si>
+  <si>
+    <t>will make</t>
+  </si>
+  <si>
+    <t>a cake</t>
+  </si>
+  <si>
+    <t>will stay</t>
+  </si>
+  <si>
+    <t>because he cares</t>
+  </si>
+  <si>
+    <t>will be</t>
+  </si>
+  <si>
+    <t>such a fun day</t>
+  </si>
+  <si>
+    <t>will go</t>
+  </si>
+  <si>
+    <t>through the tunnel</t>
+  </si>
+  <si>
+    <t>will get</t>
+  </si>
+  <si>
+    <t>a gift</t>
+  </si>
+  <si>
+    <t>will work</t>
+  </si>
+  <si>
+    <t>tomorrow</t>
+  </si>
+  <si>
+    <t>will help</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>This</t>
+  </si>
+  <si>
+    <t>a different story</t>
+  </si>
+  <si>
+    <t>сподобається</t>
+  </si>
+  <si>
+    <t>використає</t>
+  </si>
+  <si>
+    <t>зроблять</t>
+  </si>
+  <si>
+    <t>залишиться</t>
+  </si>
+  <si>
+    <t>буде</t>
+  </si>
+  <si>
+    <t>пройдемо</t>
+  </si>
+  <si>
+    <t>отримаєш</t>
+  </si>
+  <si>
+    <t>працюватиму</t>
+  </si>
+  <si>
+    <t>допоможуть</t>
+  </si>
+  <si>
+    <t>needed</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>watched</t>
+  </si>
+  <si>
+    <t>a new film</t>
+  </si>
+  <si>
+    <t>She just</t>
+  </si>
+  <si>
+    <t>arrived</t>
+  </si>
+  <si>
+    <t>He only</t>
+  </si>
+  <si>
+    <t>smiled</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>the old book</t>
+  </si>
+  <si>
+    <t>looked</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>watered</t>
+  </si>
+  <si>
+    <t>the plants</t>
+  </si>
+  <si>
+    <t>wanted</t>
+  </si>
+  <si>
+    <t>some water</t>
+  </si>
+  <si>
+    <t>called</t>
+  </si>
+  <si>
+    <t>, but no one answered</t>
+  </si>
+  <si>
+    <t>потребував</t>
+  </si>
+  <si>
+    <t>дивилися</t>
+  </si>
+  <si>
+    <t>прибув</t>
+  </si>
+  <si>
+    <t>посміхнувся</t>
+  </si>
+  <si>
+    <t>користувалися</t>
+  </si>
+  <si>
+    <t>виглядало</t>
+  </si>
+  <si>
+    <t>поливала</t>
+  </si>
+  <si>
+    <t>вивчали</t>
+  </si>
+  <si>
+    <t>хотів</t>
+  </si>
+  <si>
+    <t>дзвонили</t>
+  </si>
+  <si>
+    <t>studied</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>saw</t>
+  </si>
+  <si>
+    <t>went</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>gave</t>
+  </si>
+  <si>
+    <t>one answer</t>
+  </si>
+  <si>
+    <t>drank</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>were</t>
+  </si>
+  <si>
+    <t>very happy</t>
+  </si>
+  <si>
+    <t>had</t>
+  </si>
+  <si>
+    <t>a good time</t>
+  </si>
+  <si>
+    <t>came</t>
+  </si>
+  <si>
+    <t>early</t>
+  </si>
+  <si>
+    <t>took</t>
+  </si>
+  <si>
+    <t>some bread</t>
+  </si>
+  <si>
+    <t>thought</t>
+  </si>
+  <si>
+    <t>about that</t>
+  </si>
+  <si>
+    <t>made</t>
+  </si>
+  <si>
+    <t>a plan</t>
+  </si>
+  <si>
+    <t>дивився</t>
+  </si>
+  <si>
+    <t>пішла</t>
+  </si>
+  <si>
+    <t>дала</t>
+  </si>
+  <si>
+    <t>випили</t>
+  </si>
+  <si>
+    <t>були</t>
+  </si>
+  <si>
+    <t>мали</t>
+  </si>
+  <si>
+    <t>прийшов</t>
+  </si>
+  <si>
+    <t>взяла</t>
+  </si>
+  <si>
+    <t>думав</t>
+  </si>
+  <si>
+    <t>склали</t>
+  </si>
+  <si>
+    <t>know</t>
+  </si>
+  <si>
+    <t>the way</t>
+  </si>
+  <si>
+    <t>will feel</t>
+  </si>
+  <si>
+    <t>well</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>My friend</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>draw</t>
+  </si>
+  <si>
+    <t>will know</t>
+  </si>
+  <si>
+    <t>his name</t>
+  </si>
+  <si>
+    <t>said</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>will have</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>Then we</t>
+  </si>
+  <si>
+    <t>walked</t>
+  </si>
+  <si>
+    <t>Each child</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>art</t>
+  </si>
+  <si>
+    <t>любили</t>
+  </si>
+  <si>
+    <t>loved</t>
+  </si>
+  <si>
+    <t>знаю</t>
+  </si>
+  <si>
+    <t>почуватиметься</t>
+  </si>
+  <si>
+    <t>пішов</t>
+  </si>
+  <si>
+    <t>може</t>
+  </si>
+  <si>
+    <t>знатимеш</t>
+  </si>
+  <si>
+    <t>сказав</t>
+  </si>
+  <si>
+    <t>буде мати</t>
+  </si>
+  <si>
+    <t>пішли</t>
+  </si>
+  <si>
+    <t>is looking</t>
+  </si>
+  <si>
+    <t>at the wall</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>are travelling</t>
+  </si>
+  <si>
+    <t>around the world</t>
+  </si>
+  <si>
+    <t>is reading</t>
+  </si>
+  <si>
+    <t>a newspaper</t>
+  </si>
+  <si>
+    <t>are studing</t>
+  </si>
+  <si>
+    <t>the map now</t>
+  </si>
+  <si>
+    <t>are trying</t>
+  </si>
+  <si>
+    <t>to find the answer</t>
+  </si>
+  <si>
+    <t>am not eating</t>
+  </si>
+  <si>
+    <t>much today</t>
+  </si>
+  <si>
+    <t>is taking</t>
+  </si>
+  <si>
+    <t>a photo</t>
+  </si>
+  <si>
+    <t>is saying</t>
+  </si>
+  <si>
+    <t>he wants more food</t>
+  </si>
+  <si>
+    <t>are talking</t>
+  </si>
+  <si>
+    <t>about something important</t>
+  </si>
+  <si>
+    <t>My family</t>
+  </si>
+  <si>
+    <t>is having</t>
+  </si>
+  <si>
+    <t>dinner</t>
+  </si>
+  <si>
+    <t>дивиться</t>
+  </si>
+  <si>
+    <t>подорожують</t>
+  </si>
+  <si>
+    <t>читає</t>
+  </si>
+  <si>
+    <t>вивчають</t>
+  </si>
+  <si>
+    <t>намагаються</t>
+  </si>
+  <si>
+    <t>не їм</t>
+  </si>
+  <si>
+    <t>знімає</t>
+  </si>
+  <si>
+    <t>каже</t>
+  </si>
+  <si>
+    <t>обідає</t>
   </si>
 </sst>
 </file>
@@ -595,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB64D9CB-62E1-4E7F-A9F1-9B1326169423}">
   <dimension ref="A2:J360"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="F84" workbookViewId="0">
+      <selection activeCell="J87" sqref="J87:J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -608,7 +1211,7 @@
     <col min="5" max="5" width="12.88671875" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="5.5546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="86" style="2" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="2"/>
@@ -985,297 +1588,270 @@
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J16" s="2" t="str">
         <f>A16&amp;B16&amp;C16&amp;D16&amp;E16&amp;F16&amp;G16&amp;H16&amp;I16</f>
-        <v>{beginning: "beginning text", word: "word text2", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "", word: "Він", translat: "He", ending: "likes ice-cream"},</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J17" s="2" t="str">
         <f t="shared" ref="J17:J24" si="1">A17&amp;B17&amp;C17&amp;D17&amp;E17&amp;F17&amp;G17&amp;H17&amp;I17</f>
-        <v>{beginning: "beginning text", word: "word text3", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "", word: "Ми", translat: "We", ending: "learn English"},</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{beginning: "beginning text", word: "word text4", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "", word: "Вона", translat: "She", ending: "goes to town"},</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{beginning: "beginning text", word: "word text5", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "", word: "Ти", translat: "You", ending: "help people"},</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{beginning: "beginning text", word: "word text6", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "", word: "Вони", translat: "They", ending: "look in the window"},</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{beginning: "beginning text", word: "word text7", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "", word: "Ви", translat: "You", ending: "will find the key"},</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{beginning: "beginning text", word: "word text8", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "", word: "Воно", translat: "It", ending: "knows something"},</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{beginning: "beginning text", word: "word text9", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "", word: "Ми", translat: "We", ending: "want peace"},</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{beginning: "beginning text", word: "word text10", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "", word: "Вони", translat: "They", ending: "take our time"},</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1287,30 +1863,33 @@
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B27" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J27" s="2" t="str">
         <f>A27&amp;B27&amp;C27&amp;D27&amp;E27&amp;F27&amp;G27&amp;H27&amp;I27</f>
-        <v>{beginning: "", word: "Я", translat: "I", ending: "love Ukraine"},</v>
+        <v>{beginning: "I", word: "хочу", translat: "want", ending: "more juice"},</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1318,32 +1897,32 @@
         <v>0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J28" s="2" t="str">
         <f>A28&amp;B28&amp;C28&amp;D28&amp;E28&amp;F28&amp;G28&amp;H28&amp;I28</f>
-        <v>{beginning: "beginning text", word: "word text2", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", word: "має", translat: "has", ending: "many friends"},</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -1351,32 +1930,32 @@
         <v>0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J29" s="2" t="str">
         <f t="shared" ref="J29:J36" si="2">A29&amp;B29&amp;C29&amp;D29&amp;E29&amp;F29&amp;G29&amp;H29&amp;I29</f>
-        <v>{beginning: "beginning text", word: "word text3", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "What do you", word: "їсте", translat: "eat", ending: "?"},</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -1384,32 +1963,32 @@
         <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J30" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{beginning: "beginning text", word: "word text4", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", word: "говоримо", translat: "talk", ending: "about school"},</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -1417,32 +1996,29 @@
         <v>0</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J31" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{beginning: "beginning text", word: "word text5", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "All kids", word: "граються", translat: "play", ending: ""},</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -1450,32 +2026,32 @@
         <v>0</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J32" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{beginning: "beginning text", word: "word text6", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", word: "бігає", translat: "runs", ending: "fast"},</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -1483,32 +2059,29 @@
         <v>0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J33" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{beginning: "beginning text", word: "word text7", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "Many birds", word: "співають", translat: "sing", ending: ""},</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -1516,32 +2089,32 @@
         <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J34" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{beginning: "beginning text", word: "word text8", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "роблять", translat: "do", ending: "homework"},</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -1549,32 +2122,29 @@
         <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J35" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{beginning: "beginning text", word: "word text9", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "Most people", word: "посміхаються", translat: "smile", ending: ""},</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -1582,32 +2152,32 @@
         <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J36" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{beginning: "beginning text", word: "word text10", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "Time", word: "йде", translat: "goes", ending: "fast"},</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -1619,30 +2189,33 @@
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B39" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C39" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J39" s="2" t="str">
         <f>A39&amp;B39&amp;C39&amp;D39&amp;E39&amp;F39&amp;G39&amp;H39&amp;I39</f>
-        <v>{beginning: "", word: "Я", translat: "I", ending: "love Ukraine"},</v>
+        <v>{beginning: "I", word: "сподобається", translat: "will like", ending: "this book"},</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -1650,32 +2223,32 @@
         <v>0</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J40" s="2" t="str">
         <f>A40&amp;B40&amp;C40&amp;D40&amp;E40&amp;F40&amp;G40&amp;H40&amp;I40</f>
-        <v>{beginning: "beginning text", word: "word text2", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", word: "використає", translat: "will use", ending: "that pan"},</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -1683,32 +2256,32 @@
         <v>0</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J41" s="2" t="str">
         <f t="shared" ref="J41:J48" si="3">A41&amp;B41&amp;C41&amp;D41&amp;E41&amp;F41&amp;G41&amp;H41&amp;I41</f>
-        <v>{beginning: "beginning text", word: "word text3", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "зроблять", translat: "will make", ending: "a cake"},</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -1716,32 +2289,32 @@
         <v>0</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{beginning: "beginning text", word: "word text4", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", word: "залишиться", translat: "will stay", ending: "because he cares"},</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -1749,32 +2322,32 @@
         <v>0</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J43" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{beginning: "beginning text", word: "word text5", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "It", word: "буде", translat: "will be", ending: "such a fun day"},</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -1782,32 +2355,32 @@
         <v>0</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J44" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{beginning: "beginning text", word: "word text6", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", word: "пройдемо", translat: "will go", ending: "through the tunnel"},</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -1815,32 +2388,32 @@
         <v>0</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>17</v>
+        <v>129</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J45" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{beginning: "beginning text", word: "word text7", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "You", word: "отримаєш", translat: "will get", ending: "a gift"},</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -1848,32 +2421,32 @@
         <v>0</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J46" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{beginning: "beginning text", word: "word text8", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "I", word: "працюватиму", translat: "will work", ending: "tomorrow"},</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -1881,32 +2454,32 @@
         <v>0</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J47" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{beginning: "beginning text", word: "word text9", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "допоможуть", translat: "will help", ending: "us"},</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -1914,32 +2487,32 @@
         <v>0</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J48" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{beginning: "beginning text", word: "word text10", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "This", word: "буде", translat: "will be", ending: "a different story"},</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -1951,30 +2524,33 @@
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B51" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C51" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>12</v>
+        <v>133</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J51" s="2" t="str">
         <f>A51&amp;B51&amp;C51&amp;D51&amp;E51&amp;F51&amp;G51&amp;H51&amp;I51</f>
-        <v>{beginning: "", word: "Я", translat: "I", ending: "love Ukraine"},</v>
+        <v>{beginning: "I", word: "потребував", translat: "needed", ending: "help"},</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -1982,32 +2558,32 @@
         <v>0</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>8</v>
+        <v>151</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>4</v>
+        <v>134</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>6</v>
+        <v>135</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J52" s="2" t="str">
         <f>A52&amp;B52&amp;C52&amp;D52&amp;E52&amp;F52&amp;G52&amp;H52&amp;I52</f>
-        <v>{beginning: "beginning text", word: "word text2", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "дивилися", translat: "watched", ending: "a new film"},</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -2015,32 +2591,29 @@
         <v>0</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>13</v>
+        <v>152</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>4</v>
+        <v>137</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J53" s="2" t="str">
         <f t="shared" ref="J53:J60" si="4">A53&amp;B53&amp;C53&amp;D53&amp;E53&amp;F53&amp;G53&amp;H53&amp;I53</f>
-        <v>{beginning: "beginning text", word: "word text3", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She just", word: "прибув", translat: "arrived", ending: ""},</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -2048,32 +2621,29 @@
         <v>0</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>4</v>
+        <v>139</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J54" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", word: "word text4", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He only", word: "посміхнувся", translat: "smiled", ending: ""},</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -2081,32 +2651,32 @@
         <v>0</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>15</v>
+        <v>154</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J55" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", word: "word text5", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", word: "користувалися", translat: "used", ending: "the old book"},</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -2114,32 +2684,32 @@
         <v>0</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J56" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", word: "word text6", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "It", word: "виглядало", translat: "looked", ending: "good"},</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
@@ -2147,32 +2717,32 @@
         <v>0</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J57" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", word: "word text7", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", word: "поливала", translat: "watered", ending: "the plants"},</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
@@ -2180,32 +2750,32 @@
         <v>0</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J58" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", word: "word text8", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "вивчали", translat: "studied", ending: "history"},</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -2213,32 +2783,32 @@
         <v>0</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>19</v>
+        <v>158</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>4</v>
+        <v>146</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J59" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", word: "word text9", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", word: "хотів", translat: "wanted", ending: "some water"},</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -2246,32 +2816,32 @@
         <v>0</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>20</v>
+        <v>159</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>4</v>
+        <v>148</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>6</v>
+        <v>149</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J60" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", word: "word text10", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "I", word: "дзвонили", translat: "called", ending: ", but no one answered"},</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -2283,30 +2853,33 @@
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B63" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C63" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>12</v>
+        <v>135</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J63" s="2" t="str">
         <f>A63&amp;B63&amp;C63&amp;D63&amp;E63&amp;F63&amp;G63&amp;H63&amp;I63</f>
-        <v>{beginning: "", word: "Я", translat: "I", ending: "love Ukraine"},</v>
+        <v>{beginning: "I", word: "дивився", translat: "saw", ending: "a new film"},</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -2314,32 +2887,32 @@
         <v>0</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>8</v>
+        <v>182</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>6</v>
+        <v>164</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J64" s="2" t="str">
         <f>A64&amp;B64&amp;C64&amp;D64&amp;E64&amp;F64&amp;G64&amp;H64&amp;I64</f>
-        <v>{beginning: "beginning text", word: "word text2", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She just", word: "пішла", translat: "went", ending: "home"},</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -2347,32 +2920,32 @@
         <v>0</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>13</v>
+        <v>183</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>4</v>
+        <v>165</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J65" s="2" t="str">
         <f t="shared" ref="J65:J72" si="5">A65&amp;B65&amp;C65&amp;D65&amp;E65&amp;F65&amp;G65&amp;H65&amp;I65</f>
-        <v>{beginning: "beginning text", word: "word text3", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He only", word: "дала", translat: "gave", ending: "one answer"},</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -2380,32 +2953,32 @@
         <v>0</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>14</v>
+        <v>184</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>4</v>
+        <v>167</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J66" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", word: "word text4", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", word: "випили", translat: "drank", ending: "water"},</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
@@ -2413,32 +2986,32 @@
         <v>0</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J67" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", word: "word text5", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "були", translat: "were", ending: "very happy"},</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -2446,32 +3019,32 @@
         <v>0</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>16</v>
+        <v>186</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>4</v>
+        <v>171</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J68" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", word: "word text6", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "I", word: "мали", translat: "had", ending: "a good time"},</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
@@ -2479,32 +3052,32 @@
         <v>0</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>17</v>
+        <v>187</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J69" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", word: "word text7", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", word: "прийшов", translat: "came", ending: "early"},</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -2512,32 +3085,32 @@
         <v>0</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>18</v>
+        <v>188</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>4</v>
+        <v>175</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>6</v>
+        <v>176</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J70" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", word: "word text8", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", word: "взяла", translat: "took", ending: "some bread"},</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -2545,32 +3118,32 @@
         <v>0</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>19</v>
+        <v>189</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>4</v>
+        <v>177</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J71" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", word: "word text9", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "I", word: "думав", translat: "thought", ending: "about that"},</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -2578,32 +3151,32 @@
         <v>0</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>20</v>
+        <v>190</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>4</v>
+        <v>179</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>6</v>
+        <v>180</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J72" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", word: "word text10", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "склали", translat: "made", ending: "a plan"},</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -2615,30 +3188,33 @@
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B75" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>10</v>
+        <v>212</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>12</v>
+        <v>192</v>
       </c>
       <c r="I75" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J75" s="2" t="str">
         <f>A75&amp;B75&amp;C75&amp;D75&amp;E75&amp;F75&amp;G75&amp;H75&amp;I75</f>
-        <v>{beginning: "", word: "Я", translat: "I", ending: "love Ukraine"},</v>
+        <v>{beginning: "I", word: "знаю", translat: "know", ending: "the way"},</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
@@ -2646,32 +3222,32 @@
         <v>0</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>8</v>
+        <v>213</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J76" s="2" t="str">
         <f>A76&amp;B76&amp;C76&amp;D76&amp;E76&amp;F76&amp;G76&amp;H76&amp;I76</f>
-        <v>{beginning: "beginning text", word: "word text2", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", word: "почуватиметься", translat: "will feel", ending: "well"},</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
@@ -2679,32 +3255,32 @@
         <v>0</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>13</v>
+        <v>214</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>6</v>
+        <v>195</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J77" s="2" t="str">
         <f t="shared" ref="J77:J84" si="6">A77&amp;B77&amp;C77&amp;D77&amp;E77&amp;F77&amp;G77&amp;H77&amp;I77</f>
-        <v>{beginning: "beginning text", word: "word text3", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", word: "пішов", translat: "went", ending: "first"},</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
@@ -2712,32 +3288,32 @@
         <v>0</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1</v>
+        <v>196</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>14</v>
+        <v>215</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>6</v>
+        <v>198</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J78" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", word: "word text4", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "My friend", word: "може", translat: "can", ending: "draw"},</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
@@ -2745,32 +3321,32 @@
         <v>0</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>15</v>
+        <v>216</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>4</v>
+        <v>199</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J79" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", word: "word text5", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "You", word: "знатимеш", translat: "will know", ending: "his name"},</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
@@ -2778,32 +3354,32 @@
         <v>0</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>4</v>
+        <v>201</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>6</v>
+        <v>202</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J80" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", word: "word text6", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "I", word: "сказав", translat: "said", ending: "yes"},</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
@@ -2811,32 +3387,32 @@
         <v>0</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>17</v>
+        <v>218</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>4</v>
+        <v>203</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>6</v>
+        <v>204</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J81" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", word: "word text7", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", word: "буде мати", translat: "will have", ending: "money"},</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
@@ -2844,32 +3420,32 @@
         <v>0</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>1</v>
+        <v>205</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>18</v>
+        <v>219</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>4</v>
+        <v>206</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>6</v>
+        <v>164</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J82" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", word: "word text8", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "Then we", word: "пішли", translat: "walked", ending: "home"},</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
@@ -2877,32 +3453,32 @@
         <v>0</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>1</v>
+        <v>207</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>19</v>
+        <v>215</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J83" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", word: "word text9", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "Each child", word: "може", translat: "can", ending: "read"},</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
@@ -2910,32 +3486,32 @@
         <v>0</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>20</v>
+        <v>210</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>6</v>
+        <v>209</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J84" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", word: "word text10", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "любили", translat: "loved", ending: "art"},</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -2947,30 +3523,33 @@
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B87" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="C87" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>10</v>
+        <v>242</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>11</v>
+        <v>220</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>12</v>
+        <v>221</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J87" s="2" t="str">
         <f>A87&amp;B87&amp;C87&amp;D87&amp;E87&amp;F87&amp;G87&amp;H87&amp;I87</f>
-        <v>{beginning: "", word: "Я", translat: "I", ending: "love Ukraine"},</v>
+        <v>{beginning: "She", word: "дивиться", translat: "is looking", ending: "at the wall"},</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
@@ -2978,32 +3557,32 @@
         <v>0</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1</v>
+        <v>222</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>8</v>
+        <v>243</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>4</v>
+        <v>223</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>6</v>
+        <v>224</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J88" s="2" t="str">
         <f>A88&amp;B88&amp;C88&amp;D88&amp;E88&amp;F88&amp;G88&amp;H88&amp;I88</f>
-        <v>{beginning: "beginning text", word: "word text2", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "People", word: "подорожують", translat: "are travelling", ending: "around the world"},</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -3011,32 +3590,32 @@
         <v>0</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>13</v>
+        <v>244</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>6</v>
+        <v>226</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J89" s="2" t="str">
         <f t="shared" ref="J89:J96" si="7">A89&amp;B89&amp;C89&amp;D89&amp;E89&amp;F89&amp;G89&amp;H89&amp;I89</f>
-        <v>{beginning: "beginning text", word: "word text3", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", word: "читає", translat: "is reading", ending: "a newspaper"},</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
@@ -3044,32 +3623,32 @@
         <v>0</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>14</v>
+        <v>245</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>4</v>
+        <v>227</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>6</v>
+        <v>228</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J90" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", word: "word text4", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", word: "вивчають", translat: "are studing", ending: "the map now"},</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
@@ -3077,32 +3656,32 @@
         <v>0</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>15</v>
+        <v>246</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>4</v>
+        <v>229</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>6</v>
+        <v>230</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J91" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", word: "word text5", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "намагаються", translat: "are trying", ending: "to find the answer"},</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
@@ -3110,32 +3689,32 @@
         <v>0</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>16</v>
+        <v>247</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>4</v>
+        <v>231</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="I92" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J92" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", word: "word text6", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "I", word: "не їм", translat: "am not eating", ending: "much today"},</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
@@ -3143,32 +3722,32 @@
         <v>0</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>17</v>
+        <v>248</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>4</v>
+        <v>233</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>6</v>
+        <v>234</v>
       </c>
       <c r="I93" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J93" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", word: "word text7", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", word: "знімає", translat: "is taking", ending: "a photo"},</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
@@ -3176,32 +3755,32 @@
         <v>0</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>18</v>
+        <v>249</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>4</v>
+        <v>235</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>6</v>
+        <v>236</v>
       </c>
       <c r="I94" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J94" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", word: "word text8", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", word: "каже", translat: "is saying", ending: "he wants more food"},</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
@@ -3209,32 +3788,32 @@
         <v>0</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>4</v>
+        <v>237</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>6</v>
+        <v>238</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J95" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", word: "word text9", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", word: "говоримо", translat: "are talking", ending: "about something important"},</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
@@ -3242,32 +3821,32 @@
         <v>0</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1</v>
+        <v>239</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>4</v>
+        <v>240</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>6</v>
+        <v>241</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J96" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", word: "word text10", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "My family", word: "обідає", translat: "is having", ending: "dinner"},</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
replaceit 10 lessons completed
</commit_message>
<xml_diff>
--- a/public/docs/Grammar_replaceit_exercise.xlsx
+++ b/public/docs/Grammar_replaceit_exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C339AD-E391-44A3-AF31-DF7A91C00E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02E156E-D7FB-4E76-9D1E-22B5920CB70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1020" windowWidth="14220" windowHeight="8880" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
+    <workbookView minimized="1" xWindow="-23820" yWindow="915" windowWidth="15390" windowHeight="8880" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2692" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="301">
   <si>
     <t>{beginning: "</t>
   </si>
@@ -789,6 +789,156 @@
   </si>
   <si>
     <t>обідає</t>
+  </si>
+  <si>
+    <t>is not reading</t>
+  </si>
+  <si>
+    <t>a new book</t>
+  </si>
+  <si>
+    <t>were not keeping</t>
+  </si>
+  <si>
+    <t>the door open</t>
+  </si>
+  <si>
+    <t>will be joining</t>
+  </si>
+  <si>
+    <t>this project</t>
+  </si>
+  <si>
+    <t>is starting</t>
+  </si>
+  <si>
+    <t>a new job</t>
+  </si>
+  <si>
+    <t>was learning</t>
+  </si>
+  <si>
+    <t>a lot last year</t>
+  </si>
+  <si>
+    <t>The teacher</t>
+  </si>
+  <si>
+    <t>will be helping</t>
+  </si>
+  <si>
+    <t>every student</t>
+  </si>
+  <si>
+    <t>are working</t>
+  </si>
+  <si>
+    <t>in the field now</t>
+  </si>
+  <si>
+    <t>a large house</t>
+  </si>
+  <si>
+    <t>will be building</t>
+  </si>
+  <si>
+    <t>was calling</t>
+  </si>
+  <si>
+    <t>was making</t>
+  </si>
+  <si>
+    <t>the files available</t>
+  </si>
+  <si>
+    <t>не тримали</t>
+  </si>
+  <si>
+    <t>приєднаємося</t>
+  </si>
+  <si>
+    <t>починає</t>
+  </si>
+  <si>
+    <t>вивчав</t>
+  </si>
+  <si>
+    <t>допомагатиме</t>
+  </si>
+  <si>
+    <t>працюють</t>
+  </si>
+  <si>
+    <t>будемо будувати</t>
+  </si>
+  <si>
+    <t>кликала</t>
+  </si>
+  <si>
+    <t>зробив</t>
+  </si>
+  <si>
+    <t>have lived</t>
+  </si>
+  <si>
+    <t>here for 10 years</t>
+  </si>
+  <si>
+    <t>We both</t>
+  </si>
+  <si>
+    <t>have worked</t>
+  </si>
+  <si>
+    <t>here since Summer</t>
+  </si>
+  <si>
+    <t>have given</t>
+  </si>
+  <si>
+    <t>us the keys</t>
+  </si>
+  <si>
+    <t>Scientists</t>
+  </si>
+  <si>
+    <t>have studied</t>
+  </si>
+  <si>
+    <t>human behaviour for centuries</t>
+  </si>
+  <si>
+    <t>Both teams</t>
+  </si>
+  <si>
+    <t>have played</t>
+  </si>
+  <si>
+    <t>has searched</t>
+  </si>
+  <si>
+    <t>for it since last week</t>
+  </si>
+  <si>
+    <t>without the car for a month</t>
+  </si>
+  <si>
+    <t>has found</t>
+  </si>
+  <si>
+    <t>something interesting</t>
+  </si>
+  <si>
+    <t>have come</t>
+  </si>
+  <si>
+    <t>to visit us</t>
+  </si>
+  <si>
+    <t>have met</t>
+  </si>
+  <si>
+    <t>the local guide</t>
   </si>
 </sst>
 </file>
@@ -1198,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB64D9CB-62E1-4E7F-A9F1-9B1326169423}">
   <dimension ref="A2:J360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F84" workbookViewId="0">
-      <selection activeCell="J87" sqref="J87:J96"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3858,30 +4008,33 @@
       <c r="A99" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B99" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="C99" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>10</v>
+        <v>244</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>11</v>
+        <v>251</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>12</v>
+        <v>252</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J99" s="2" t="str">
         <f>A99&amp;B99&amp;C99&amp;D99&amp;E99&amp;F99&amp;G99&amp;H99&amp;I99</f>
-        <v>{beginning: "", word: "Я", translat: "I", ending: "love Ukraine"},</v>
+        <v>{beginning: "She", word: "читає", translat: "is not reading", ending: "a new book"},</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
@@ -3889,32 +4042,32 @@
         <v>0</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>8</v>
+        <v>271</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>6</v>
+        <v>254</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J100" s="2" t="str">
         <f>A100&amp;B100&amp;C100&amp;D100&amp;E100&amp;F100&amp;G100&amp;H100&amp;I100</f>
-        <v>{beginning: "beginning text", word: "word text2", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "не тримали", translat: "were not keeping", ending: "the door open"},</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
@@ -3922,32 +4075,32 @@
         <v>0</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>13</v>
+        <v>272</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>4</v>
+        <v>255</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>6</v>
+        <v>256</v>
       </c>
       <c r="I101" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J101" s="2" t="str">
         <f t="shared" ref="J101:J108" si="8">A101&amp;B101&amp;C101&amp;D101&amp;E101&amp;F101&amp;G101&amp;H101&amp;I101</f>
-        <v>{beginning: "beginning text", word: "word text3", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", word: "приєднаємося", translat: "will be joining", ending: "this project"},</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
@@ -3955,32 +4108,32 @@
         <v>0</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>14</v>
+        <v>273</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>4</v>
+        <v>257</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>6</v>
+        <v>258</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J102" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", word: "word text4", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", word: "починає", translat: "is starting", ending: "a new job"},</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
@@ -3988,32 +4141,32 @@
         <v>0</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>15</v>
+        <v>274</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>6</v>
+        <v>260</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J103" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", word: "word text5", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "I", word: "вивчав", translat: "was learning", ending: "a lot last year"},</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
@@ -4021,32 +4174,32 @@
         <v>0</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>1</v>
+        <v>261</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>16</v>
+        <v>275</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>4</v>
+        <v>262</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>6</v>
+        <v>263</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J104" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", word: "word text6", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "The teacher", word: "допомагатиме", translat: "will be helping", ending: "every student"},</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
@@ -4054,32 +4207,32 @@
         <v>0</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>17</v>
+        <v>276</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>4</v>
+        <v>264</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J105" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", word: "word text7", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "працюють", translat: "are working", ending: "in the field now"},</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
@@ -4087,32 +4240,32 @@
         <v>0</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>18</v>
+        <v>277</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>4</v>
+        <v>267</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>6</v>
+        <v>266</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J106" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", word: "word text8", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", word: "будемо будувати", translat: "will be building", ending: "a large house"},</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
@@ -4120,32 +4273,32 @@
         <v>0</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>19</v>
+        <v>278</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>4</v>
+        <v>268</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="I107" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J107" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", word: "word text9", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", word: "кликала", translat: "was calling", ending: "us"},</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
@@ -4153,32 +4306,32 @@
         <v>0</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>20</v>
+        <v>279</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>4</v>
+        <v>269</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>6</v>
+        <v>270</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J108" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", word: "word text10", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", word: "зробив", translat: "was making", ending: "the files available"},</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
@@ -4190,6 +4343,9 @@
       <c r="A111" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B111" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C111" s="2" t="s">
         <v>2</v>
       </c>
@@ -4200,20 +4356,20 @@
         <v>3</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>11</v>
+        <v>280</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>12</v>
+        <v>281</v>
       </c>
       <c r="I111" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J111" s="2" t="str">
         <f>A111&amp;B111&amp;C111&amp;D111&amp;E111&amp;F111&amp;G111&amp;H111&amp;I111</f>
-        <v>{beginning: "", word: "Я", translat: "I", ending: "love Ukraine"},</v>
+        <v>{beginning: "I", word: "Я", translat: "have lived", ending: "here for 10 years"},</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
@@ -4221,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>1</v>
+        <v>282</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>2</v>
@@ -4233,20 +4389,20 @@
         <v>3</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>4</v>
+        <v>283</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>6</v>
+        <v>284</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J112" s="2" t="str">
         <f>A112&amp;B112&amp;C112&amp;D112&amp;E112&amp;F112&amp;G112&amp;H112&amp;I112</f>
-        <v>{beginning: "beginning text", word: "word text2", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We both", word: "word text2", translat: "have worked", ending: "here since Summer"},</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
@@ -4254,7 +4410,7 @@
         <v>0</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>2</v>
@@ -4266,20 +4422,20 @@
         <v>3</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>4</v>
+        <v>285</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>6</v>
+        <v>286</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J113" s="2" t="str">
         <f t="shared" ref="J113:J120" si="9">A113&amp;B113&amp;C113&amp;D113&amp;E113&amp;F113&amp;G113&amp;H113&amp;I113</f>
-        <v>{beginning: "beginning text", word: "word text3", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "word text3", translat: "have given", ending: "us the keys"},</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
@@ -4287,7 +4443,7 @@
         <v>0</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>1</v>
+        <v>287</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>2</v>
@@ -4299,20 +4455,20 @@
         <v>3</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>4</v>
+        <v>288</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>6</v>
+        <v>289</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J114" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>{beginning: "beginning text", word: "word text4", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "Scientists", word: "word text4", translat: "have studied", ending: "human behaviour for centuries"},</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
@@ -4320,7 +4476,7 @@
         <v>0</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>1</v>
+        <v>290</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>2</v>
@@ -4332,20 +4488,20 @@
         <v>3</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>4</v>
+        <v>291</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J115" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>{beginning: "beginning text", word: "word text5", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "Both teams", word: "word text5", translat: "have played", ending: "well"},</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
@@ -4353,7 +4509,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>2</v>
@@ -4365,20 +4521,20 @@
         <v>3</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>4</v>
+        <v>292</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>6</v>
+        <v>293</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J116" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>{beginning: "beginning text", word: "word text6", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", word: "word text6", translat: "has searched", ending: "for it since last week"},</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
@@ -4386,7 +4542,7 @@
         <v>0</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>2</v>
@@ -4398,20 +4554,20 @@
         <v>3</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>4</v>
+        <v>280</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>6</v>
+        <v>294</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J117" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>{beginning: "beginning text", word: "word text7", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", word: "word text7", translat: "have lived", ending: "without the car for a month"},</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
@@ -4419,7 +4575,7 @@
         <v>0</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>2</v>
@@ -4431,20 +4587,20 @@
         <v>3</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>4</v>
+        <v>295</v>
       </c>
       <c r="G118" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>6</v>
+        <v>296</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J118" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>{beginning: "beginning text", word: "word text8", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", word: "word text8", translat: "has found", ending: "something interesting"},</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
@@ -4452,7 +4608,7 @@
         <v>0</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>2</v>
@@ -4464,20 +4620,20 @@
         <v>3</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>4</v>
+        <v>297</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>6</v>
+        <v>298</v>
       </c>
       <c r="I119" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J119" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>{beginning: "beginning text", word: "word text9", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", word: "word text9", translat: "have come", ending: "to visit us"},</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
@@ -4485,7 +4641,7 @@
         <v>0</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>2</v>
@@ -4497,20 +4653,20 @@
         <v>3</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>4</v>
+        <v>299</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>6</v>
+        <v>300</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J120" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>{beginning: "beginning text", word: "word text10", translat: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", word: "word text10", translat: "have met", ending: "the local guide"},</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>